<commit_message>
renaming trc file creation module
</commit_message>
<xml_diff>
--- a/FMC_to_trc/OpenSimInputFiles/compare mediapipe_opensim_pose2sim.xlsx
+++ b/FMC_to_trc/OpenSimInputFiles/compare mediapipe_opensim_pose2sim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Prible\Box\Research\FMC_projects\FMC_to_trc\OpenSimInputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944D56C-E4FA-4ED9-8F7E-DA5657709F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0B81FE-B274-4768-AE75-8C00D57F6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
   <si>
     <t>RHip</t>
   </si>
@@ -648,18 +648,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D78"/>
+  <dimension ref="B3:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -667,15 +668,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -683,7 +687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -691,23 +695,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -715,7 +725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -723,7 +733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -731,7 +741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -739,71 +749,101 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -811,7 +851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -819,7 +859,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -827,7 +867,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -835,122 +875,146 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>67</v>
       </c>

</xml_diff>